<commit_message>
Initial changes from BMS hardware review
Added CAN transceiver and finished some of the recommendations from the review
</commit_message>
<xml_diff>
--- a/STM32F405 & LTC6820 Test Board/STM32-LTC6820 BOM.xlsx
+++ b/STM32F405 & LTC6820 Test Board/STM32-LTC6820 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Waterloop\electrical-BMS\STM32F405 &amp; LTC6820 Test Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2A67EA-3664-4AD2-94E3-53C42C955F26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19587138-44FE-42D2-954C-0FAAE25C4F5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ED85FC06-DFEA-4137-BEB4-927617E32267}"/>
+    <workbookView xWindow="5808" yWindow="1764" windowWidth="17280" windowHeight="8964" xr2:uid="{ED85FC06-DFEA-4137-BEB4-927617E32267}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="96">
   <si>
     <t>Designator</t>
   </si>
@@ -72,9 +74,6 @@
     <t>399-6951-1-ND</t>
   </si>
   <si>
-    <t>C3, C4, C5, C6, C13</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.1µF ±10% 10V Ceramic Capacitor X7R 0805 (2012 Metric) </t>
   </si>
   <si>
@@ -129,9 +128,6 @@
     <t>P1, P2</t>
   </si>
   <si>
-    <t>P3, P4</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -309,32 +305,30 @@
     <t>1253-1373-1-ND</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>1/1 Transceiver Half CANbus 8-SO</t>
+  </si>
+  <si>
+    <t>TJA1051T/3/CM,118</t>
+  </si>
+  <si>
+    <t>568-11885-1-ND</t>
+  </si>
+  <si>
+    <t>C3, C4, C5, C6, C13, C14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -376,17 +370,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,7 +697,7 @@
   <dimension ref="B2:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,19 +764,19 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -792,25 +785,25 @@
         <v>0.3</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I23" si="0">G4*H4</f>
+        <f t="shared" ref="I4:I24" si="0">G4*H4</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -825,19 +818,19 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -852,19 +845,19 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -879,19 +872,19 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
         <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -906,19 +899,19 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
         <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -933,10 +926,10 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D10" s="4">
         <v>61303211121</v>
@@ -945,7 +938,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -960,46 +953,46 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
       <c r="G11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>0.18</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>0.36</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
         <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1014,19 +1007,19 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
         <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>61</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -1041,19 +1034,19 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
         <v>62</v>
-      </c>
-      <c r="D14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>64</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -1068,19 +1061,19 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
         <v>65</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>67</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1095,19 +1088,19 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
         <v>68</v>
-      </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>70</v>
       </c>
       <c r="G16">
         <v>4</v>
@@ -1122,19 +1115,19 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
         <v>71</v>
-      </c>
-      <c r="D17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>73</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1149,19 +1142,19 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
         <v>74</v>
-      </c>
-      <c r="D18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
-        <v>76</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1176,19 +1169,19 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
         <v>77</v>
-      </c>
-      <c r="D19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>79</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1203,19 +1196,19 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
         <v>80</v>
-      </c>
-      <c r="D20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>82</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1230,46 +1223,46 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
         <v>83</v>
       </c>
-      <c r="D21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" t="s">
-        <v>85</v>
-      </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21">
-        <v>18.260000000000002</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>18.260000000000002</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
         <v>86</v>
-      </c>
-      <c r="D22" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" t="s">
-        <v>88</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1284,19 +1277,19 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
         <v>89</v>
-      </c>
-      <c r="D23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" t="s">
-        <v>91</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1310,9 +1303,30 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I24" s="5">
-        <f>SUM(I3:I23)</f>
-        <v>50.660000000000004</v>
+      <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1.58</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>1.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM and shcematic PDF have been added
title
</commit_message>
<xml_diff>
--- a/STM32F405 & LTC6820 Test Board/STM32-LTC6820 BOM.xlsx
+++ b/STM32F405 & LTC6820 Test Board/STM32-LTC6820 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Waterloop\electrical-BMS\STM32F405 &amp; LTC6820 Test Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19587138-44FE-42D2-954C-0FAAE25C4F5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B034B848-D15E-41C7-99D5-EBCFAE5B642F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5808" yWindow="1764" windowWidth="17280" windowHeight="8964" xr2:uid="{ED85FC06-DFEA-4137-BEB4-927617E32267}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ED85FC06-DFEA-4137-BEB4-927617E32267}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -137,9 +137,6 @@
     <t>R4</t>
   </si>
   <si>
-    <t>R5, R8, R9, R10</t>
-  </si>
-  <si>
     <t>R7</t>
   </si>
   <si>
@@ -320,14 +317,17 @@
     <t>568-11885-1-ND</t>
   </si>
   <si>
-    <t>C3, C4, C5, C6, C13, C14</t>
+    <t>C3, C4, C5, C6, C13, C14, C15</t>
+  </si>
+  <si>
+    <t>R5, R8, R9, R10, R12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +345,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -370,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -380,6 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{178C6A52-931E-4DFB-BB29-A3BF94BEDADC}">
-  <dimension ref="B2:I24"/>
+  <dimension ref="B2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,7 +773,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -779,14 +788,14 @@
         <v>15</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H4">
         <v>0.3</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I24" si="0">G4*H4</f>
-        <v>1.5</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
@@ -875,16 +884,16 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
         <v>42</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
         <v>43</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" t="s">
-        <v>44</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -902,16 +911,16 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
         <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -929,7 +938,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="4">
         <v>61303211121</v>
@@ -938,7 +947,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -953,19 +962,19 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
         <v>49</v>
-      </c>
-      <c r="E11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" t="s">
-        <v>50</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -983,16 +992,16 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
         <v>53</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
         <v>54</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>55</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1007,19 +1016,19 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
         <v>56</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>57</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
         <v>58</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>59</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -1037,16 +1046,16 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
         <v>60</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
         <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>62</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -1064,16 +1073,16 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
         <v>63</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" t="s">
-        <v>65</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -1088,46 +1097,46 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s">
         <v>66</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
         <v>67</v>
       </c>
-      <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>68</v>
-      </c>
       <c r="G16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H16">
         <v>0.16</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>0.64</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
         <v>69</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
         <v>70</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>71</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1142,19 +1151,19 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
         <v>72</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
         <v>73</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
-        <v>74</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1169,19 +1178,19 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
         <v>75</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
         <v>76</v>
-      </c>
-      <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>77</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1196,19 +1205,19 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" t="s">
         <v>78</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
         <v>79</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>80</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1223,19 +1232,19 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
         <v>81</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
         <v>82</v>
-      </c>
-      <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" t="s">
-        <v>83</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1250,19 +1259,19 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" t="s">
         <v>84</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
         <v>85</v>
-      </c>
-      <c r="E22" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" t="s">
-        <v>86</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1277,19 +1286,19 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" t="s">
         <v>87</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
         <v>88</v>
-      </c>
-      <c r="E23" t="s">
-        <v>11</v>
-      </c>
-      <c r="F23" t="s">
-        <v>89</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1304,19 +1313,19 @@
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" t="s">
         <v>91</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>92</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
         <v>93</v>
-      </c>
-      <c r="E24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" t="s">
-        <v>94</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1327,6 +1336,12 @@
       <c r="I24">
         <f t="shared" si="0"/>
         <v>1.58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I25" s="5">
+        <f>SUM(I3:I24)</f>
+        <v>50.959999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial revisions to MCU schematics
Initial revision to schematics to make them more readable + get rid of unecessary sheets
</commit_message>
<xml_diff>
--- a/STM32F405 & LTC6820 Test Board/STM32-LTC6820 BOM.xlsx
+++ b/STM32F405 & LTC6820 Test Board/STM32-LTC6820 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Waterloop\electrical-BMS\STM32F405 &amp; LTC6820 Test Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B034B848-D15E-41C7-99D5-EBCFAE5B642F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D3F11D-3EAB-48CD-B344-FBA45A2C0C43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ED85FC06-DFEA-4137-BEB4-927617E32267}"/>
   </bookViews>
@@ -706,7 +706,7 @@
   <dimension ref="B2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>